<commit_message>
Keep the original joint_id in imputated datasets; fixed the inconsistency in sample size before and after imputation.
</commit_message>
<xml_diff>
--- a/data/8 cohorts codebook.xlsx
+++ b/data/8 cohorts codebook.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JGUO258\Documents\JGUO\papers repo\diabetes_subphenotypes_predictors\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC58024D-EFF0-4D2A-B013-0EA96D776522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A883EB0F-77A5-437D-A9AB-8683EC68D51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="96">
   <si>
     <t xml:space="preserve">Harmonized </t>
   </si>
@@ -216,9 +228,6 @@
     <t>cigr_st,smk_st</t>
   </si>
   <si>
-    <t>smk_cig,smk_pipe,smk_tob</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -261,20 +270,68 @@
     <t>dppos</t>
   </si>
   <si>
-    <t>anti-depressant</t>
-  </si>
-  <si>
     <t>race_clean</t>
   </si>
   <si>
     <t>urinealbumin/urinecreatinine</t>
+  </si>
+  <si>
+    <t>med_chol_now</t>
+  </si>
+  <si>
+    <t>med_dep_now</t>
+  </si>
+  <si>
+    <t>med_diab</t>
+  </si>
+  <si>
+    <t>med_hbp_now, med_hbp_ever</t>
+  </si>
+  <si>
+    <t>smk_evr,smk_cur</t>
+  </si>
+  <si>
+    <t>dmmedsins</t>
+  </si>
+  <si>
+    <t>dmmedsoral,dmmedsins,dmmeds</t>
+  </si>
+  <si>
+    <t>med_statins</t>
+  </si>
+  <si>
+    <t>med_statins,med_statins_self,med_statins_past</t>
+  </si>
+  <si>
+    <t>med_bp_past,med_bp,med_bp_self</t>
+  </si>
+  <si>
+    <t>med_dep_past</t>
+  </si>
+  <si>
+    <t>med_dep_use</t>
+  </si>
+  <si>
+    <t>med_bp</t>
+  </si>
+  <si>
+    <t>med_dep</t>
+  </si>
+  <si>
+    <t>med_lipid,med_statins</t>
+  </si>
+  <si>
+    <t>smk,smk_cig,smk_pipe,smk_tob</t>
+  </si>
+  <si>
+    <t>smk_cur,smk_evr,smk_cig,smk_pip</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,8 +368,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFEE0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,6 +419,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -368,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -395,7 +465,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -708,17 +780,17 @@
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>77</v>
+      <c r="H1" s="20" t="s">
+        <v>76</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>10</v>
@@ -726,7 +798,7 @@
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="11">
         <v>601</v>
@@ -758,7 +830,7 @@
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="12">
         <v>22925</v>
@@ -853,7 +925,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>46</v>
@@ -890,10 +962,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -954,22 +1026,22 @@
         <v>14</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H11" t="s">
         <v>54</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1032,7 +1104,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
@@ -1076,16 +1148,16 @@
         <v>62</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>45</v>
+        <v>94</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>95</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -1114,99 +1186,131 @@
         <v>45</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17" s="16"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" t="s">
-        <v>76</v>
+      <c r="A18" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F18" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" t="s">
-        <v>76</v>
-      </c>
-      <c r="H18" t="s">
-        <v>76</v>
-      </c>
-      <c r="I18" t="s">
-        <v>76</v>
+        <v>87</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" t="s">
         <v>74</v>
       </c>
       <c r="D19" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="I19" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" t="s">
-        <v>75</v>
+      <c r="A20" s="21" t="s">
+        <v>90</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>80</v>
+      </c>
+      <c r="F20" t="s">
+        <v>89</v>
       </c>
       <c r="G20" t="s">
-        <v>75</v>
-      </c>
-      <c r="I20" t="s">
-        <v>75</v>
+        <v>92</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="10"/>
+        <v>75</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21" t="s">
+        <v>75</v>
+      </c>
+      <c r="I21" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E22" s="10"/>
+      <c r="F22" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E23" s="10"/>
+      <c r="F23" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E24" s="10"/>
     </row>
@@ -1753,7 +1857,7 @@
         <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E45" t="s">
         <v>38</v>
@@ -1787,8 +1891,8 @@
       <c r="E46" t="s">
         <v>39</v>
       </c>
-      <c r="F46" s="20" t="s">
-        <v>80</v>
+      <c r="F46" t="s">
+        <v>78</v>
       </c>
       <c r="G46" t="s">
         <v>39</v>

</xml_diff>